<commit_message>
run table by dict_header_qres
</commit_message>
<xml_diff>
--- a/tests/VN8413_Data_preview.xlsx
+++ b/tests/VN8413_Data_preview.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BU151"/>
+  <dimension ref="A1:BV151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -795,6 +795,11 @@
           <t>New_MA_6</t>
         </is>
       </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_Var</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -994,6 +999,9 @@
       <c r="BS2" t="inlineStr"/>
       <c r="BT2" t="inlineStr"/>
       <c r="BU2" t="inlineStr"/>
+      <c r="BV2" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -1197,6 +1205,9 @@
       <c r="BS3" t="inlineStr"/>
       <c r="BT3" t="inlineStr"/>
       <c r="BU3" t="inlineStr"/>
+      <c r="BV3" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -1400,6 +1411,9 @@
       <c r="BS4" t="inlineStr"/>
       <c r="BT4" t="inlineStr"/>
       <c r="BU4" t="inlineStr"/>
+      <c r="BV4" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -1601,6 +1615,9 @@
       <c r="BS5" t="inlineStr"/>
       <c r="BT5" t="inlineStr"/>
       <c r="BU5" t="inlineStr"/>
+      <c r="BV5" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1804,6 +1821,9 @@
       <c r="BS6" t="inlineStr"/>
       <c r="BT6" t="inlineStr"/>
       <c r="BU6" t="inlineStr"/>
+      <c r="BV6" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1999,6 +2019,9 @@
       <c r="BS7" t="inlineStr"/>
       <c r="BT7" t="inlineStr"/>
       <c r="BU7" t="inlineStr"/>
+      <c r="BV7" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -2200,6 +2223,9 @@
       <c r="BS8" t="inlineStr"/>
       <c r="BT8" t="inlineStr"/>
       <c r="BU8" t="inlineStr"/>
+      <c r="BV8" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -2401,6 +2427,9 @@
       <c r="BS9" t="inlineStr"/>
       <c r="BT9" t="inlineStr"/>
       <c r="BU9" t="inlineStr"/>
+      <c r="BV9" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -2604,6 +2633,9 @@
       <c r="BS10" t="inlineStr"/>
       <c r="BT10" t="inlineStr"/>
       <c r="BU10" t="inlineStr"/>
+      <c r="BV10" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -2801,6 +2833,9 @@
       <c r="BS11" t="inlineStr"/>
       <c r="BT11" t="inlineStr"/>
       <c r="BU11" t="inlineStr"/>
+      <c r="BV11" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -2996,6 +3031,9 @@
       <c r="BS12" t="inlineStr"/>
       <c r="BT12" t="inlineStr"/>
       <c r="BU12" t="inlineStr"/>
+      <c r="BV12" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -3197,6 +3235,9 @@
       <c r="BS13" t="inlineStr"/>
       <c r="BT13" t="inlineStr"/>
       <c r="BU13" t="inlineStr"/>
+      <c r="BV13" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -3392,6 +3433,9 @@
       <c r="BS14" t="inlineStr"/>
       <c r="BT14" t="inlineStr"/>
       <c r="BU14" t="inlineStr"/>
+      <c r="BV14" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -3593,6 +3637,9 @@
       <c r="BS15" t="inlineStr"/>
       <c r="BT15" t="inlineStr"/>
       <c r="BU15" t="inlineStr"/>
+      <c r="BV15" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -3796,6 +3843,9 @@
       <c r="BS16" t="inlineStr"/>
       <c r="BT16" t="inlineStr"/>
       <c r="BU16" t="inlineStr"/>
+      <c r="BV16" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -3999,6 +4049,9 @@
       <c r="BS17" t="inlineStr"/>
       <c r="BT17" t="inlineStr"/>
       <c r="BU17" t="inlineStr"/>
+      <c r="BV17" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -4196,6 +4249,9 @@
       <c r="BS18" t="inlineStr"/>
       <c r="BT18" t="inlineStr"/>
       <c r="BU18" t="inlineStr"/>
+      <c r="BV18" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -4395,6 +4451,9 @@
       <c r="BS19" t="inlineStr"/>
       <c r="BT19" t="inlineStr"/>
       <c r="BU19" t="inlineStr"/>
+      <c r="BV19" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -4592,6 +4651,9 @@
       <c r="BS20" t="inlineStr"/>
       <c r="BT20" t="inlineStr"/>
       <c r="BU20" t="inlineStr"/>
+      <c r="BV20" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -4795,6 +4857,9 @@
       <c r="BS21" t="inlineStr"/>
       <c r="BT21" t="inlineStr"/>
       <c r="BU21" t="inlineStr"/>
+      <c r="BV21" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -5000,6 +5065,9 @@
       <c r="BS22" t="inlineStr"/>
       <c r="BT22" t="inlineStr"/>
       <c r="BU22" t="inlineStr"/>
+      <c r="BV22" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -5201,6 +5269,9 @@
       <c r="BS23" t="inlineStr"/>
       <c r="BT23" t="inlineStr"/>
       <c r="BU23" t="inlineStr"/>
+      <c r="BV23" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -5400,6 +5471,9 @@
       <c r="BS24" t="inlineStr"/>
       <c r="BT24" t="inlineStr"/>
       <c r="BU24" t="inlineStr"/>
+      <c r="BV24" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -5603,6 +5677,9 @@
       <c r="BS25" t="inlineStr"/>
       <c r="BT25" t="inlineStr"/>
       <c r="BU25" t="inlineStr"/>
+      <c r="BV25" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -5802,6 +5879,9 @@
       <c r="BS26" t="inlineStr"/>
       <c r="BT26" t="inlineStr"/>
       <c r="BU26" t="inlineStr"/>
+      <c r="BV26" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -6003,6 +6083,9 @@
       <c r="BS27" t="inlineStr"/>
       <c r="BT27" t="inlineStr"/>
       <c r="BU27" t="inlineStr"/>
+      <c r="BV27" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -6208,6 +6291,9 @@
       <c r="BS28" t="inlineStr"/>
       <c r="BT28" t="inlineStr"/>
       <c r="BU28" t="inlineStr"/>
+      <c r="BV28" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -6411,6 +6497,9 @@
       <c r="BS29" t="inlineStr"/>
       <c r="BT29" t="inlineStr"/>
       <c r="BU29" t="inlineStr"/>
+      <c r="BV29" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -6614,6 +6703,9 @@
       <c r="BS30" t="inlineStr"/>
       <c r="BT30" t="inlineStr"/>
       <c r="BU30" t="inlineStr"/>
+      <c r="BV30" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -6817,6 +6909,9 @@
       <c r="BS31" t="inlineStr"/>
       <c r="BT31" t="inlineStr"/>
       <c r="BU31" t="inlineStr"/>
+      <c r="BV31" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -7016,6 +7111,9 @@
       <c r="BS32" t="inlineStr"/>
       <c r="BT32" t="inlineStr"/>
       <c r="BU32" t="inlineStr"/>
+      <c r="BV32" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -7219,6 +7317,9 @@
       <c r="BS33" t="inlineStr"/>
       <c r="BT33" t="inlineStr"/>
       <c r="BU33" t="inlineStr"/>
+      <c r="BV33" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -7420,6 +7521,9 @@
       <c r="BS34" t="inlineStr"/>
       <c r="BT34" t="inlineStr"/>
       <c r="BU34" t="inlineStr"/>
+      <c r="BV34" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -7623,6 +7727,9 @@
       <c r="BS35" t="inlineStr"/>
       <c r="BT35" t="inlineStr"/>
       <c r="BU35" t="inlineStr"/>
+      <c r="BV35" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -7826,6 +7933,9 @@
       <c r="BS36" t="inlineStr"/>
       <c r="BT36" t="inlineStr"/>
       <c r="BU36" t="inlineStr"/>
+      <c r="BV36" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -8025,6 +8135,9 @@
       <c r="BS37" t="inlineStr"/>
       <c r="BT37" t="inlineStr"/>
       <c r="BU37" t="inlineStr"/>
+      <c r="BV37" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -8228,6 +8341,9 @@
       <c r="BS38" t="inlineStr"/>
       <c r="BT38" t="inlineStr"/>
       <c r="BU38" t="inlineStr"/>
+      <c r="BV38" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -8429,6 +8545,9 @@
       <c r="BS39" t="inlineStr"/>
       <c r="BT39" t="inlineStr"/>
       <c r="BU39" t="inlineStr"/>
+      <c r="BV39" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -8626,6 +8745,9 @@
       <c r="BS40" t="inlineStr"/>
       <c r="BT40" t="inlineStr"/>
       <c r="BU40" t="inlineStr"/>
+      <c r="BV40" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -8825,6 +8947,9 @@
       <c r="BS41" t="inlineStr"/>
       <c r="BT41" t="inlineStr"/>
       <c r="BU41" t="inlineStr"/>
+      <c r="BV41" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -9026,6 +9151,9 @@
       <c r="BS42" t="inlineStr"/>
       <c r="BT42" t="inlineStr"/>
       <c r="BU42" t="inlineStr"/>
+      <c r="BV42" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -9225,6 +9353,9 @@
       <c r="BS43" t="inlineStr"/>
       <c r="BT43" t="inlineStr"/>
       <c r="BU43" t="inlineStr"/>
+      <c r="BV43" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -9428,6 +9559,9 @@
       <c r="BS44" t="inlineStr"/>
       <c r="BT44" t="inlineStr"/>
       <c r="BU44" t="inlineStr"/>
+      <c r="BV44" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -9627,6 +9761,9 @@
       <c r="BS45" t="inlineStr"/>
       <c r="BT45" t="inlineStr"/>
       <c r="BU45" t="inlineStr"/>
+      <c r="BV45" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -9830,6 +9967,9 @@
       <c r="BS46" t="inlineStr"/>
       <c r="BT46" t="inlineStr"/>
       <c r="BU46" t="inlineStr"/>
+      <c r="BV46" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -10033,6 +10173,9 @@
       <c r="BS47" t="inlineStr"/>
       <c r="BT47" t="inlineStr"/>
       <c r="BU47" t="inlineStr"/>
+      <c r="BV47" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -10234,6 +10377,9 @@
       <c r="BS48" t="inlineStr"/>
       <c r="BT48" t="inlineStr"/>
       <c r="BU48" t="inlineStr"/>
+      <c r="BV48" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -10437,6 +10583,9 @@
       <c r="BS49" t="inlineStr"/>
       <c r="BT49" t="inlineStr"/>
       <c r="BU49" t="inlineStr"/>
+      <c r="BV49" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -10638,6 +10787,9 @@
       <c r="BS50" t="inlineStr"/>
       <c r="BT50" t="inlineStr"/>
       <c r="BU50" t="inlineStr"/>
+      <c r="BV50" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -10841,6 +10993,9 @@
       <c r="BS51" t="inlineStr"/>
       <c r="BT51" t="inlineStr"/>
       <c r="BU51" t="inlineStr"/>
+      <c r="BV51" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -11044,6 +11199,9 @@
       <c r="BS52" t="inlineStr"/>
       <c r="BT52" t="inlineStr"/>
       <c r="BU52" t="inlineStr"/>
+      <c r="BV52" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -11247,6 +11405,9 @@
       <c r="BS53" t="inlineStr"/>
       <c r="BT53" t="inlineStr"/>
       <c r="BU53" t="inlineStr"/>
+      <c r="BV53" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -11448,6 +11609,9 @@
       <c r="BS54" t="inlineStr"/>
       <c r="BT54" t="inlineStr"/>
       <c r="BU54" t="inlineStr"/>
+      <c r="BV54" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -11651,6 +11815,9 @@
       <c r="BS55" t="inlineStr"/>
       <c r="BT55" t="inlineStr"/>
       <c r="BU55" t="inlineStr"/>
+      <c r="BV55" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -11854,6 +12021,9 @@
       <c r="BS56" t="inlineStr"/>
       <c r="BT56" t="inlineStr"/>
       <c r="BU56" t="inlineStr"/>
+      <c r="BV56" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -12055,6 +12225,9 @@
       <c r="BS57" t="inlineStr"/>
       <c r="BT57" t="inlineStr"/>
       <c r="BU57" t="inlineStr"/>
+      <c r="BV57" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -12258,6 +12431,9 @@
       <c r="BS58" t="inlineStr"/>
       <c r="BT58" t="inlineStr"/>
       <c r="BU58" t="inlineStr"/>
+      <c r="BV58" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -12461,6 +12637,9 @@
       <c r="BS59" t="inlineStr"/>
       <c r="BT59" t="inlineStr"/>
       <c r="BU59" t="inlineStr"/>
+      <c r="BV59" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -12664,6 +12843,9 @@
       <c r="BS60" t="inlineStr"/>
       <c r="BT60" t="inlineStr"/>
       <c r="BU60" t="inlineStr"/>
+      <c r="BV60" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -12867,6 +13049,9 @@
       <c r="BS61" t="inlineStr"/>
       <c r="BT61" t="inlineStr"/>
       <c r="BU61" t="inlineStr"/>
+      <c r="BV61" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -13066,6 +13251,9 @@
       <c r="BS62" t="inlineStr"/>
       <c r="BT62" t="inlineStr"/>
       <c r="BU62" t="inlineStr"/>
+      <c r="BV62" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -13263,6 +13451,9 @@
       <c r="BS63" t="inlineStr"/>
       <c r="BT63" t="inlineStr"/>
       <c r="BU63" t="inlineStr"/>
+      <c r="BV63" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -13466,6 +13657,9 @@
       <c r="BS64" t="inlineStr"/>
       <c r="BT64" t="inlineStr"/>
       <c r="BU64" t="inlineStr"/>
+      <c r="BV64" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -13665,6 +13859,9 @@
       <c r="BS65" t="inlineStr"/>
       <c r="BT65" t="inlineStr"/>
       <c r="BU65" t="inlineStr"/>
+      <c r="BV65" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -13866,6 +14063,9 @@
       <c r="BS66" t="inlineStr"/>
       <c r="BT66" t="inlineStr"/>
       <c r="BU66" t="inlineStr"/>
+      <c r="BV66" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -14069,6 +14269,9 @@
       <c r="BS67" t="inlineStr"/>
       <c r="BT67" t="inlineStr"/>
       <c r="BU67" t="inlineStr"/>
+      <c r="BV67" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -14264,6 +14467,9 @@
       <c r="BS68" t="inlineStr"/>
       <c r="BT68" t="inlineStr"/>
       <c r="BU68" t="inlineStr"/>
+      <c r="BV68" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -14467,6 +14673,9 @@
       <c r="BS69" t="inlineStr"/>
       <c r="BT69" t="inlineStr"/>
       <c r="BU69" t="inlineStr"/>
+      <c r="BV69" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -14668,6 +14877,9 @@
       <c r="BS70" t="inlineStr"/>
       <c r="BT70" t="inlineStr"/>
       <c r="BU70" t="inlineStr"/>
+      <c r="BV70" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -14871,6 +15083,9 @@
       <c r="BS71" t="inlineStr"/>
       <c r="BT71" t="inlineStr"/>
       <c r="BU71" t="inlineStr"/>
+      <c r="BV71" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -15074,6 +15289,9 @@
       <c r="BS72" t="inlineStr"/>
       <c r="BT72" t="inlineStr"/>
       <c r="BU72" t="inlineStr"/>
+      <c r="BV72" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -15277,6 +15495,9 @@
       <c r="BS73" t="inlineStr"/>
       <c r="BT73" t="inlineStr"/>
       <c r="BU73" t="inlineStr"/>
+      <c r="BV73" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -15480,6 +15701,9 @@
       <c r="BS74" t="inlineStr"/>
       <c r="BT74" t="inlineStr"/>
       <c r="BU74" t="inlineStr"/>
+      <c r="BV74" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -15683,6 +15907,9 @@
       <c r="BS75" t="inlineStr"/>
       <c r="BT75" t="inlineStr"/>
       <c r="BU75" t="inlineStr"/>
+      <c r="BV75" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -15886,6 +16113,9 @@
       <c r="BS76" t="inlineStr"/>
       <c r="BT76" t="inlineStr"/>
       <c r="BU76" t="inlineStr"/>
+      <c r="BV76" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -16085,6 +16315,9 @@
       <c r="BS77" t="inlineStr"/>
       <c r="BT77" t="inlineStr"/>
       <c r="BU77" t="inlineStr"/>
+      <c r="BV77" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -16286,6 +16519,9 @@
       <c r="BS78" t="inlineStr"/>
       <c r="BT78" t="inlineStr"/>
       <c r="BU78" t="inlineStr"/>
+      <c r="BV78" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -16485,6 +16721,9 @@
       <c r="BS79" t="inlineStr"/>
       <c r="BT79" t="inlineStr"/>
       <c r="BU79" t="inlineStr"/>
+      <c r="BV79" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -16688,6 +16927,9 @@
       <c r="BS80" t="inlineStr"/>
       <c r="BT80" t="inlineStr"/>
       <c r="BU80" t="inlineStr"/>
+      <c r="BV80" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -16883,6 +17125,9 @@
       <c r="BS81" t="inlineStr"/>
       <c r="BT81" t="inlineStr"/>
       <c r="BU81" t="inlineStr"/>
+      <c r="BV81" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -17084,6 +17329,9 @@
       <c r="BS82" t="inlineStr"/>
       <c r="BT82" t="inlineStr"/>
       <c r="BU82" t="inlineStr"/>
+      <c r="BV82" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -17287,6 +17535,9 @@
       <c r="BS83" t="inlineStr"/>
       <c r="BT83" t="inlineStr"/>
       <c r="BU83" t="inlineStr"/>
+      <c r="BV83" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -17488,6 +17739,9 @@
       <c r="BS84" t="inlineStr"/>
       <c r="BT84" t="inlineStr"/>
       <c r="BU84" t="inlineStr"/>
+      <c r="BV84" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -17689,6 +17943,9 @@
       <c r="BS85" t="inlineStr"/>
       <c r="BT85" t="inlineStr"/>
       <c r="BU85" t="inlineStr"/>
+      <c r="BV85" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -17890,6 +18147,9 @@
       <c r="BS86" t="inlineStr"/>
       <c r="BT86" t="inlineStr"/>
       <c r="BU86" t="inlineStr"/>
+      <c r="BV86" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -18091,6 +18351,9 @@
       <c r="BS87" t="inlineStr"/>
       <c r="BT87" t="inlineStr"/>
       <c r="BU87" t="inlineStr"/>
+      <c r="BV87" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -18292,6 +18555,9 @@
       <c r="BS88" t="inlineStr"/>
       <c r="BT88" t="inlineStr"/>
       <c r="BU88" t="inlineStr"/>
+      <c r="BV88" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -18491,6 +18757,9 @@
       <c r="BS89" t="inlineStr"/>
       <c r="BT89" t="inlineStr"/>
       <c r="BU89" t="inlineStr"/>
+      <c r="BV89" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -18692,6 +18961,9 @@
       <c r="BS90" t="inlineStr"/>
       <c r="BT90" t="inlineStr"/>
       <c r="BU90" t="inlineStr"/>
+      <c r="BV90" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -18893,6 +19165,9 @@
       <c r="BS91" t="inlineStr"/>
       <c r="BT91" t="inlineStr"/>
       <c r="BU91" t="inlineStr"/>
+      <c r="BV91" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -19096,6 +19371,9 @@
       <c r="BS92" t="inlineStr"/>
       <c r="BT92" t="inlineStr"/>
       <c r="BU92" t="inlineStr"/>
+      <c r="BV92" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -19295,6 +19573,9 @@
       <c r="BS93" t="inlineStr"/>
       <c r="BT93" t="inlineStr"/>
       <c r="BU93" t="inlineStr"/>
+      <c r="BV93" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -19494,6 +19775,9 @@
       <c r="BS94" t="inlineStr"/>
       <c r="BT94" t="inlineStr"/>
       <c r="BU94" t="inlineStr"/>
+      <c r="BV94" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -19693,6 +19977,9 @@
       <c r="BS95" t="inlineStr"/>
       <c r="BT95" t="inlineStr"/>
       <c r="BU95" t="inlineStr"/>
+      <c r="BV95" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -19896,6 +20183,9 @@
       <c r="BS96" t="inlineStr"/>
       <c r="BT96" t="inlineStr"/>
       <c r="BU96" t="inlineStr"/>
+      <c r="BV96" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -20095,6 +20385,9 @@
       <c r="BS97" t="inlineStr"/>
       <c r="BT97" t="inlineStr"/>
       <c r="BU97" t="inlineStr"/>
+      <c r="BV97" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -20294,6 +20587,9 @@
       <c r="BS98" t="inlineStr"/>
       <c r="BT98" t="inlineStr"/>
       <c r="BU98" t="inlineStr"/>
+      <c r="BV98" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -20493,6 +20789,9 @@
       <c r="BS99" t="inlineStr"/>
       <c r="BT99" t="inlineStr"/>
       <c r="BU99" t="inlineStr"/>
+      <c r="BV99" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -20694,6 +20993,9 @@
       <c r="BS100" t="inlineStr"/>
       <c r="BT100" t="inlineStr"/>
       <c r="BU100" t="inlineStr"/>
+      <c r="BV100" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -20895,6 +21197,9 @@
       <c r="BS101" t="inlineStr"/>
       <c r="BT101" t="inlineStr"/>
       <c r="BU101" t="inlineStr"/>
+      <c r="BV101" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -21094,6 +21399,9 @@
       <c r="BS102" t="inlineStr"/>
       <c r="BT102" t="inlineStr"/>
       <c r="BU102" t="inlineStr"/>
+      <c r="BV102" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -21295,6 +21603,9 @@
       <c r="BS103" t="inlineStr"/>
       <c r="BT103" t="inlineStr"/>
       <c r="BU103" t="inlineStr"/>
+      <c r="BV103" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -21496,6 +21807,9 @@
       <c r="BS104" t="inlineStr"/>
       <c r="BT104" t="inlineStr"/>
       <c r="BU104" t="inlineStr"/>
+      <c r="BV104" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -21695,6 +22009,9 @@
       <c r="BS105" t="inlineStr"/>
       <c r="BT105" t="inlineStr"/>
       <c r="BU105" t="inlineStr"/>
+      <c r="BV105" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -21892,6 +22209,9 @@
       <c r="BS106" t="inlineStr"/>
       <c r="BT106" t="inlineStr"/>
       <c r="BU106" t="inlineStr"/>
+      <c r="BV106" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -22093,6 +22413,9 @@
       <c r="BS107" t="inlineStr"/>
       <c r="BT107" t="inlineStr"/>
       <c r="BU107" t="inlineStr"/>
+      <c r="BV107" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -22294,6 +22617,9 @@
       <c r="BS108" t="inlineStr"/>
       <c r="BT108" t="inlineStr"/>
       <c r="BU108" t="inlineStr"/>
+      <c r="BV108" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -22495,6 +22821,9 @@
       <c r="BS109" t="inlineStr"/>
       <c r="BT109" t="inlineStr"/>
       <c r="BU109" t="inlineStr"/>
+      <c r="BV109" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -22696,6 +23025,9 @@
       <c r="BS110" t="inlineStr"/>
       <c r="BT110" t="inlineStr"/>
       <c r="BU110" t="inlineStr"/>
+      <c r="BV110" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -22897,6 +23229,9 @@
       <c r="BS111" t="inlineStr"/>
       <c r="BT111" t="inlineStr"/>
       <c r="BU111" t="inlineStr"/>
+      <c r="BV111" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -23096,6 +23431,9 @@
       <c r="BS112" t="inlineStr"/>
       <c r="BT112" t="inlineStr"/>
       <c r="BU112" t="inlineStr"/>
+      <c r="BV112" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -23299,6 +23637,9 @@
       <c r="BS113" t="inlineStr"/>
       <c r="BT113" t="inlineStr"/>
       <c r="BU113" t="inlineStr"/>
+      <c r="BV113" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -23504,6 +23845,9 @@
       <c r="BS114" t="inlineStr"/>
       <c r="BT114" t="inlineStr"/>
       <c r="BU114" t="inlineStr"/>
+      <c r="BV114" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -23705,6 +24049,9 @@
       <c r="BS115" t="inlineStr"/>
       <c r="BT115" t="inlineStr"/>
       <c r="BU115" t="inlineStr"/>
+      <c r="BV115" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -23904,6 +24251,9 @@
       <c r="BS116" t="inlineStr"/>
       <c r="BT116" t="inlineStr"/>
       <c r="BU116" t="inlineStr"/>
+      <c r="BV116" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -24105,6 +24455,9 @@
       <c r="BS117" t="inlineStr"/>
       <c r="BT117" t="inlineStr"/>
       <c r="BU117" t="inlineStr"/>
+      <c r="BV117" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -24308,6 +24661,9 @@
       <c r="BS118" t="inlineStr"/>
       <c r="BT118" t="inlineStr"/>
       <c r="BU118" t="inlineStr"/>
+      <c r="BV118" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -24507,6 +24863,9 @@
       <c r="BS119" t="inlineStr"/>
       <c r="BT119" t="inlineStr"/>
       <c r="BU119" t="inlineStr"/>
+      <c r="BV119" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -24706,6 +25065,9 @@
       <c r="BS120" t="inlineStr"/>
       <c r="BT120" t="inlineStr"/>
       <c r="BU120" t="inlineStr"/>
+      <c r="BV120" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -24907,6 +25269,9 @@
       <c r="BS121" t="inlineStr"/>
       <c r="BT121" t="inlineStr"/>
       <c r="BU121" t="inlineStr"/>
+      <c r="BV121" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -25108,6 +25473,9 @@
       <c r="BS122" t="inlineStr"/>
       <c r="BT122" t="inlineStr"/>
       <c r="BU122" t="inlineStr"/>
+      <c r="BV122" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -25311,6 +25679,9 @@
       <c r="BS123" t="inlineStr"/>
       <c r="BT123" t="inlineStr"/>
       <c r="BU123" t="inlineStr"/>
+      <c r="BV123" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -25510,6 +25881,9 @@
       <c r="BS124" t="inlineStr"/>
       <c r="BT124" t="inlineStr"/>
       <c r="BU124" t="inlineStr"/>
+      <c r="BV124" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -25711,6 +26085,9 @@
       <c r="BS125" t="inlineStr"/>
       <c r="BT125" t="inlineStr"/>
       <c r="BU125" t="inlineStr"/>
+      <c r="BV125" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -25912,6 +26289,9 @@
       <c r="BS126" t="inlineStr"/>
       <c r="BT126" t="inlineStr"/>
       <c r="BU126" t="inlineStr"/>
+      <c r="BV126" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -26117,6 +26497,9 @@
       <c r="BS127" t="inlineStr"/>
       <c r="BT127" t="inlineStr"/>
       <c r="BU127" t="inlineStr"/>
+      <c r="BV127" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -26320,6 +26703,9 @@
       <c r="BS128" t="inlineStr"/>
       <c r="BT128" t="inlineStr"/>
       <c r="BU128" t="inlineStr"/>
+      <c r="BV128" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -26521,6 +26907,9 @@
       <c r="BS129" t="inlineStr"/>
       <c r="BT129" t="inlineStr"/>
       <c r="BU129" t="inlineStr"/>
+      <c r="BV129" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -26724,6 +27113,9 @@
       <c r="BS130" t="inlineStr"/>
       <c r="BT130" t="inlineStr"/>
       <c r="BU130" t="inlineStr"/>
+      <c r="BV130" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -26927,6 +27319,9 @@
       <c r="BS131" t="inlineStr"/>
       <c r="BT131" t="inlineStr"/>
       <c r="BU131" t="inlineStr"/>
+      <c r="BV131" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -27126,6 +27521,9 @@
       <c r="BS132" t="inlineStr"/>
       <c r="BT132" t="inlineStr"/>
       <c r="BU132" t="inlineStr"/>
+      <c r="BV132" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -27325,6 +27723,9 @@
       <c r="BS133" t="inlineStr"/>
       <c r="BT133" t="inlineStr"/>
       <c r="BU133" t="inlineStr"/>
+      <c r="BV133" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -27524,6 +27925,9 @@
       <c r="BS134" t="inlineStr"/>
       <c r="BT134" t="inlineStr"/>
       <c r="BU134" t="inlineStr"/>
+      <c r="BV134" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -27723,6 +28127,9 @@
       <c r="BS135" t="inlineStr"/>
       <c r="BT135" t="inlineStr"/>
       <c r="BU135" t="inlineStr"/>
+      <c r="BV135" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -27926,6 +28333,9 @@
       <c r="BS136" t="inlineStr"/>
       <c r="BT136" t="inlineStr"/>
       <c r="BU136" t="inlineStr"/>
+      <c r="BV136" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -28121,6 +28531,9 @@
       <c r="BS137" t="inlineStr"/>
       <c r="BT137" t="inlineStr"/>
       <c r="BU137" t="inlineStr"/>
+      <c r="BV137" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -28320,6 +28733,9 @@
       <c r="BS138" t="inlineStr"/>
       <c r="BT138" t="inlineStr"/>
       <c r="BU138" t="inlineStr"/>
+      <c r="BV138" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -28521,6 +28937,9 @@
       <c r="BS139" t="inlineStr"/>
       <c r="BT139" t="inlineStr"/>
       <c r="BU139" t="inlineStr"/>
+      <c r="BV139" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -28720,6 +29139,9 @@
       <c r="BS140" t="inlineStr"/>
       <c r="BT140" t="inlineStr"/>
       <c r="BU140" t="inlineStr"/>
+      <c r="BV140" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -28923,6 +29345,9 @@
       <c r="BS141" t="inlineStr"/>
       <c r="BT141" t="inlineStr"/>
       <c r="BU141" t="inlineStr"/>
+      <c r="BV141" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -29122,6 +29547,9 @@
       <c r="BS142" t="inlineStr"/>
       <c r="BT142" t="inlineStr"/>
       <c r="BU142" t="inlineStr"/>
+      <c r="BV142" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -29321,6 +29749,9 @@
       <c r="BS143" t="inlineStr"/>
       <c r="BT143" t="inlineStr"/>
       <c r="BU143" t="inlineStr"/>
+      <c r="BV143" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -29520,6 +29951,9 @@
       <c r="BS144" t="inlineStr"/>
       <c r="BT144" t="inlineStr"/>
       <c r="BU144" t="inlineStr"/>
+      <c r="BV144" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -29721,6 +30155,9 @@
       <c r="BS145" t="inlineStr"/>
       <c r="BT145" t="inlineStr"/>
       <c r="BU145" t="inlineStr"/>
+      <c r="BV145" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -29924,6 +30361,9 @@
       <c r="BS146" t="inlineStr"/>
       <c r="BT146" t="inlineStr"/>
       <c r="BU146" t="inlineStr"/>
+      <c r="BV146" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -30123,6 +30563,9 @@
       <c r="BS147" t="inlineStr"/>
       <c r="BT147" t="inlineStr"/>
       <c r="BU147" t="inlineStr"/>
+      <c r="BV147" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -30322,6 +30765,9 @@
       <c r="BS148" t="inlineStr"/>
       <c r="BT148" t="inlineStr"/>
       <c r="BU148" t="inlineStr"/>
+      <c r="BV148" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -30523,6 +30969,9 @@
       <c r="BS149" t="inlineStr"/>
       <c r="BT149" t="inlineStr"/>
       <c r="BU149" t="inlineStr"/>
+      <c r="BV149" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -30728,6 +31177,9 @@
       <c r="BS150" t="inlineStr"/>
       <c r="BT150" t="inlineStr"/>
       <c r="BU150" t="inlineStr"/>
+      <c r="BV150" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -30931,6 +31383,9 @@
       <c r="BS151" t="inlineStr"/>
       <c r="BT151" t="inlineStr"/>
       <c r="BU151" t="inlineStr"/>
+      <c r="BV151" t="n">
+        <v>0.3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -30943,7 +31398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -32773,6 +33228,31 @@
         </is>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Weight_Var</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Weight_Var</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>NUM</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix run ma_comb with net_code
</commit_message>
<xml_diff>
--- a/tests/VN8413_Data_preview.xlsx
+++ b/tests/VN8413_Data_preview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="df_data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="df_info" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="df_data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="df_info" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -8987,7 +8987,7 @@
       <c r="AC41" t="inlineStr"/>
       <c r="AD41" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="AE41" t="n">

</xml_diff>